<commit_message>
refactor : example.xlsx file
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongdaeyong/study/JavaProject-POI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E17A38D0-6709-CE48-A506-DA2E3BA617E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F322FF7-88D9-3B45-B973-5A21C680B100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" xr2:uid="{88664455-44CA-6444-930C-BAB3813CD71E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,26 @@
   </si>
   <si>
     <t>Song</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-03-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-03-21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-03-22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-03-23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-03-24</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -128,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -468,10 +488,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1">
@@ -542,20 +565,20 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2">
-        <v>45005</v>
-      </c>
-      <c r="B5" s="2">
-        <v>45006</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45007</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45008</v>
-      </c>
-      <c r="E5" s="2">
-        <v>45009</v>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>